<commit_message>
more data + categories from excel
</commit_message>
<xml_diff>
--- a/FCR_Template.xlsx
+++ b/FCR_Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="135" yWindow="2730" windowWidth="20175" windowHeight="7965"/>
@@ -11,12 +11,15 @@
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
     <sheet name="Φύλλο3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t>AvWeight</t>
   </si>
@@ -52,6 +55,9 @@
   </si>
   <si>
     <t>AvgCategory</t>
+  </si>
+  <si>
+    <t>100-150</t>
   </si>
 </sst>
 </file>
@@ -130,8 +136,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -427,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,6 +825,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>96</v>
+      </c>
+      <c r="B26" s="3">
+        <v>22</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1.23</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>103</v>
+      </c>
+      <c r="B27" s="3">
+        <v>18</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>120</v>
+      </c>
+      <c r="B28" s="3">
+        <v>13</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -798,10 +874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">AVERAGE(A3,B3)</f>
+        <f t="shared" ref="D3:D7" si="0">AVERAGE(A3,B3)</f>
         <v>6</v>
       </c>
     </row>
@@ -901,34 +977,19 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A7" s="1">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1">
+        <v>150</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>